<commit_message>
KETEC SiPM 263k results
</commit_message>
<xml_diff>
--- a/dV.xlsx
+++ b/dV.xlsx
@@ -376,11 +376,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="108569728"/>
-        <c:axId val="108571264"/>
+        <c:axId val="67873024"/>
+        <c:axId val="67891200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108569728"/>
+        <c:axId val="67873024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -390,12 +390,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108571264"/>
+        <c:crossAx val="67891200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108571264"/>
+        <c:axId val="67891200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -408,7 +408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108569728"/>
+        <c:crossAx val="67873024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1170,11 +1170,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109232896"/>
-        <c:axId val="109234432"/>
+        <c:axId val="81405440"/>
+        <c:axId val="81406976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109232896"/>
+        <c:axId val="81405440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="69.5"/>
@@ -1186,12 +1186,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109234432"/>
+        <c:crossAx val="81406976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109234432"/>
+        <c:axId val="81406976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1204,7 +1204,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109232896"/>
+        <c:crossAx val="81405440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1337,11 +1337,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109512960"/>
-        <c:axId val="109518848"/>
+        <c:axId val="81435648"/>
+        <c:axId val="81445632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109512960"/>
+        <c:axId val="81435648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1351,12 +1351,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109518848"/>
+        <c:crossAx val="81445632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109518848"/>
+        <c:axId val="81445632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1367,7 +1367,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109512960"/>
+        <c:crossAx val="81435648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1500,11 +1500,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109535232"/>
-        <c:axId val="109536768"/>
+        <c:axId val="83890944"/>
+        <c:axId val="83892480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109535232"/>
+        <c:axId val="83890944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1514,12 +1514,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109536768"/>
+        <c:crossAx val="83892480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109536768"/>
+        <c:axId val="83892480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1530,7 +1530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109535232"/>
+        <c:crossAx val="83890944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1663,11 +1663,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109581824"/>
-        <c:axId val="109583360"/>
+        <c:axId val="83900672"/>
+        <c:axId val="83918848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109581824"/>
+        <c:axId val="83900672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1677,12 +1677,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109583360"/>
+        <c:crossAx val="83918848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109583360"/>
+        <c:axId val="83918848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,7 +1693,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109581824"/>
+        <c:crossAx val="83900672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2477,11 +2477,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109634304"/>
-        <c:axId val="109635840"/>
+        <c:axId val="84039168"/>
+        <c:axId val="84040704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109634304"/>
+        <c:axId val="84039168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2491,12 +2491,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109635840"/>
+        <c:crossAx val="84040704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109635840"/>
+        <c:axId val="84040704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -2509,14 +2509,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109634304"/>
+        <c:crossAx val="84039168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3123,11 +3122,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109767680"/>
-        <c:axId val="109781760"/>
+        <c:axId val="84135936"/>
+        <c:axId val="84137472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109767680"/>
+        <c:axId val="84135936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3137,12 +3136,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109781760"/>
+        <c:crossAx val="84137472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109781760"/>
+        <c:axId val="84137472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="55"/>
@@ -3154,14 +3153,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109767680"/>
+        <c:crossAx val="84135936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3191,7 +3189,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3289,11 +3286,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109805952"/>
-        <c:axId val="109807488"/>
+        <c:axId val="84165760"/>
+        <c:axId val="84167296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109805952"/>
+        <c:axId val="84165760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3303,12 +3300,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109807488"/>
+        <c:crossAx val="84167296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109807488"/>
+        <c:axId val="84167296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20"/>
@@ -3320,14 +3317,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109805952"/>
+        <c:crossAx val="84165760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3357,7 +3353,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3455,11 +3450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109823872"/>
-        <c:axId val="109825408"/>
+        <c:axId val="84195968"/>
+        <c:axId val="84205952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109823872"/>
+        <c:axId val="84195968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3469,12 +3464,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109825408"/>
+        <c:crossAx val="84205952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109825408"/>
+        <c:axId val="84205952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-1500"/>
@@ -3486,14 +3481,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109823872"/>
+        <c:crossAx val="84195968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3620,11 +3614,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109833600"/>
-        <c:axId val="109864064"/>
+        <c:axId val="84685184"/>
+        <c:axId val="84686720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109833600"/>
+        <c:axId val="84685184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3634,12 +3628,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109864064"/>
+        <c:crossAx val="84686720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109864064"/>
+        <c:axId val="84686720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3650,7 +3644,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109833600"/>
+        <c:crossAx val="84685184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4358,11 +4352,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109981056"/>
-        <c:axId val="110015616"/>
+        <c:axId val="84316544"/>
+        <c:axId val="84318080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109981056"/>
+        <c:axId val="84316544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -4374,12 +4368,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110015616"/>
+        <c:crossAx val="84318080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110015616"/>
+        <c:axId val="84318080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -4392,14 +4386,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109981056"/>
+        <c:crossAx val="84316544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4550,11 +4543,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="108690432"/>
-        <c:axId val="108696320"/>
+        <c:axId val="67387776"/>
+        <c:axId val="67389312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108690432"/>
+        <c:axId val="67387776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4564,12 +4557,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108696320"/>
+        <c:crossAx val="67389312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108696320"/>
+        <c:axId val="67389312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -4582,7 +4575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108690432"/>
+        <c:crossAx val="67387776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5160,11 +5153,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="110974464"/>
-        <c:axId val="110976000"/>
+        <c:axId val="84420864"/>
+        <c:axId val="84422656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110974464"/>
+        <c:axId val="84420864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5174,12 +5167,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110976000"/>
+        <c:crossAx val="84422656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110976000"/>
+        <c:axId val="84422656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="45"/>
@@ -5191,14 +5184,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110974464"/>
+        <c:crossAx val="84420864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5228,7 +5220,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5323,11 +5314,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="111016576"/>
-        <c:axId val="111083904"/>
+        <c:axId val="84430208"/>
+        <c:axId val="84460672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="111016576"/>
+        <c:axId val="84430208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5337,12 +5328,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111083904"/>
+        <c:crossAx val="84460672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="111083904"/>
+        <c:axId val="84460672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5353,14 +5344,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111016576"/>
+        <c:crossAx val="84430208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5390,7 +5380,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5485,11 +5474,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="111100288"/>
-        <c:axId val="111101824"/>
+        <c:axId val="84546688"/>
+        <c:axId val="84548224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="111100288"/>
+        <c:axId val="84546688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5499,12 +5488,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111101824"/>
+        <c:crossAx val="84548224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="111101824"/>
+        <c:axId val="84548224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-900"/>
@@ -5517,14 +5506,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111100288"/>
+        <c:crossAx val="84546688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5651,11 +5639,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="111114112"/>
-        <c:axId val="111115648"/>
+        <c:axId val="84576896"/>
+        <c:axId val="84586880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="111114112"/>
+        <c:axId val="84576896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5665,12 +5653,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111115648"/>
+        <c:crossAx val="84586880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="111115648"/>
+        <c:axId val="84586880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="68"/>
@@ -5682,7 +5670,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111114112"/>
+        <c:crossAx val="84576896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6312,11 +6300,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124367232"/>
-        <c:axId val="124368768"/>
+        <c:axId val="84644992"/>
+        <c:axId val="84646528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124367232"/>
+        <c:axId val="84644992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70.5"/>
@@ -6328,12 +6316,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124368768"/>
+        <c:crossAx val="84646528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124368768"/>
+        <c:axId val="84646528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -6346,14 +6334,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124367232"/>
+        <c:crossAx val="84644992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7107,11 +7094,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124411904"/>
-        <c:axId val="124413440"/>
+        <c:axId val="84849408"/>
+        <c:axId val="84850944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124411904"/>
+        <c:axId val="84849408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7121,12 +7108,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124413440"/>
+        <c:crossAx val="84850944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124413440"/>
+        <c:axId val="84850944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="45"/>
@@ -7138,14 +7125,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124411904"/>
+        <c:crossAx val="84849408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7783,11 +7769,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124852480"/>
-        <c:axId val="124854272"/>
+        <c:axId val="84872192"/>
+        <c:axId val="84878080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124852480"/>
+        <c:axId val="84872192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7797,12 +7783,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124854272"/>
+        <c:crossAx val="84878080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124854272"/>
+        <c:axId val="84878080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -7815,7 +7801,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124852480"/>
+        <c:crossAx val="84872192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7828,7 +7814,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8525,11 +8510,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124912768"/>
-        <c:axId val="124914304"/>
+        <c:axId val="84866944"/>
+        <c:axId val="84868480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124912768"/>
+        <c:axId val="84866944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8539,12 +8524,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124914304"/>
+        <c:crossAx val="84868480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124914304"/>
+        <c:axId val="84868480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="45"/>
@@ -8556,14 +8541,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124912768"/>
+        <c:crossAx val="84866944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8690,11 +8674,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124938496"/>
-        <c:axId val="124944384"/>
+        <c:axId val="84917248"/>
+        <c:axId val="85144320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124938496"/>
+        <c:axId val="84917248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8704,12 +8688,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124944384"/>
+        <c:crossAx val="85144320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124944384"/>
+        <c:axId val="85144320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="37"/>
@@ -8722,7 +8706,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124938496"/>
+        <c:crossAx val="84917248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8855,11 +8839,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124960768"/>
-        <c:axId val="124962304"/>
+        <c:axId val="84951808"/>
+        <c:axId val="84953344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124960768"/>
+        <c:axId val="84951808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8869,12 +8853,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124962304"/>
+        <c:crossAx val="84953344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124962304"/>
+        <c:axId val="84953344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8885,7 +8869,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124960768"/>
+        <c:crossAx val="84951808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9533,11 +9517,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="108765184"/>
-        <c:axId val="108766720"/>
+        <c:axId val="67789952"/>
+        <c:axId val="67791488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108765184"/>
+        <c:axId val="67789952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9547,12 +9531,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108766720"/>
+        <c:crossAx val="67791488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108766720"/>
+        <c:axId val="67791488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -9564,7 +9548,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108765184"/>
+        <c:crossAx val="67789952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9698,11 +9682,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125056512"/>
-        <c:axId val="125058048"/>
+        <c:axId val="84961536"/>
+        <c:axId val="84983808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125056512"/>
+        <c:axId val="84961536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9712,12 +9696,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125058048"/>
+        <c:crossAx val="84983808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125058048"/>
+        <c:axId val="84983808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9728,7 +9712,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125056512"/>
+        <c:crossAx val="84961536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10456,11 +10440,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125134336"/>
-        <c:axId val="125135872"/>
+        <c:axId val="85121280"/>
+        <c:axId val="85458944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125134336"/>
+        <c:axId val="85121280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="71.5"/>
@@ -10472,12 +10456,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125135872"/>
+        <c:crossAx val="85458944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125135872"/>
+        <c:axId val="85458944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -10490,14 +10474,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125134336"/>
+        <c:crossAx val="85121280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10943,11 +10926,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125205120"/>
-        <c:axId val="125219200"/>
+        <c:axId val="85204352"/>
+        <c:axId val="85226624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125205120"/>
+        <c:axId val="85204352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10957,12 +10940,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125219200"/>
+        <c:crossAx val="85226624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125219200"/>
+        <c:axId val="85226624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="22"/>
@@ -10974,7 +10957,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125205120"/>
+        <c:crossAx val="85204352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11417,11 +11400,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125381632"/>
-        <c:axId val="125395712"/>
+        <c:axId val="85254144"/>
+        <c:axId val="85255680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125381632"/>
+        <c:axId val="85254144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11431,12 +11414,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125395712"/>
+        <c:crossAx val="85255680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125395712"/>
+        <c:axId val="85255680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11447,7 +11430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125381632"/>
+        <c:crossAx val="85254144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12599,11 +12582,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="108835584"/>
-        <c:axId val="108837504"/>
+        <c:axId val="67987328"/>
+        <c:axId val="68001792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108835584"/>
+        <c:axId val="67987328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12613,12 +12596,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108837504"/>
+        <c:crossAx val="68001792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108837504"/>
+        <c:axId val="68001792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -12630,7 +12613,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108835584"/>
+        <c:crossAx val="67987328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12753,11 +12736,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="108845696"/>
-        <c:axId val="108851584"/>
+        <c:axId val="69533696"/>
+        <c:axId val="69535232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108845696"/>
+        <c:axId val="69533696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12767,12 +12750,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108851584"/>
+        <c:crossAx val="69535232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108851584"/>
+        <c:axId val="69535232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12783,7 +12766,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108845696"/>
+        <c:crossAx val="69533696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12906,11 +12889,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109007232"/>
-        <c:axId val="109008768"/>
+        <c:axId val="69547520"/>
+        <c:axId val="69549056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109007232"/>
+        <c:axId val="69547520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12920,12 +12903,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109008768"/>
+        <c:crossAx val="69549056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109008768"/>
+        <c:axId val="69549056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12936,7 +12919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109007232"/>
+        <c:crossAx val="69547520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13058,11 +13041,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109029248"/>
-        <c:axId val="109030784"/>
+        <c:axId val="69577344"/>
+        <c:axId val="69583232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109029248"/>
+        <c:axId val="69577344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13072,12 +13055,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109030784"/>
+        <c:crossAx val="69583232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109030784"/>
+        <c:axId val="69583232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13088,7 +13071,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109029248"/>
+        <c:crossAx val="69577344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13813,11 +13796,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109128320"/>
-        <c:axId val="109134208"/>
+        <c:axId val="74222976"/>
+        <c:axId val="74241152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109128320"/>
+        <c:axId val="74222976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="69"/>
@@ -13829,12 +13812,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109134208"/>
+        <c:crossAx val="74241152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109134208"/>
+        <c:axId val="74241152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -13847,7 +13830,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109128320"/>
+        <c:crossAx val="74222976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14503,11 +14486,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109163648"/>
-        <c:axId val="109165184"/>
+        <c:axId val="74585984"/>
+        <c:axId val="74587520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109163648"/>
+        <c:axId val="74585984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14517,12 +14500,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109165184"/>
+        <c:crossAx val="74587520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109165184"/>
+        <c:axId val="74587520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
@@ -14534,14 +14517,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109163648"/>
+        <c:crossAx val="74585984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15873,7 +15855,7 @@
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16831,8 +16813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17629,8 +17611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="M4" workbookViewId="0">
-      <selection activeCell="AA31" sqref="AA31"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17992,8 +17974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18351,7 +18333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -18702,8 +18684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Hamamatsu add processing results
</commit_message>
<xml_diff>
--- a/dV.xlsx
+++ b/dV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="17">
   <si>
     <t>T</t>
   </si>
@@ -376,11 +376,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67873024"/>
-        <c:axId val="67891200"/>
+        <c:axId val="117200768"/>
+        <c:axId val="117202304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67873024"/>
+        <c:axId val="117200768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -390,12 +390,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67891200"/>
+        <c:crossAx val="117202304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67891200"/>
+        <c:axId val="117202304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -408,7 +408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67873024"/>
+        <c:crossAx val="117200768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1170,11 +1170,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81405440"/>
-        <c:axId val="81406976"/>
+        <c:axId val="120960512"/>
+        <c:axId val="120962048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81405440"/>
+        <c:axId val="120960512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="69.5"/>
@@ -1186,12 +1186,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81406976"/>
+        <c:crossAx val="120962048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81406976"/>
+        <c:axId val="120962048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1204,13 +1204,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81405440"/>
+        <c:crossAx val="120960512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1240,6 +1241,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1337,11 +1339,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81435648"/>
-        <c:axId val="81445632"/>
+        <c:axId val="121117696"/>
+        <c:axId val="121127680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81435648"/>
+        <c:axId val="121117696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1351,12 +1353,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81445632"/>
+        <c:crossAx val="121127680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81445632"/>
+        <c:axId val="121127680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1367,13 +1369,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81435648"/>
+        <c:crossAx val="121117696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1403,6 +1406,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1500,11 +1504,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83890944"/>
-        <c:axId val="83892480"/>
+        <c:axId val="121307904"/>
+        <c:axId val="121309440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83890944"/>
+        <c:axId val="121307904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1514,12 +1518,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83892480"/>
+        <c:crossAx val="121309440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83892480"/>
+        <c:axId val="121309440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1530,13 +1534,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83890944"/>
+        <c:crossAx val="121307904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1566,6 +1571,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1663,11 +1669,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83900672"/>
-        <c:axId val="83918848"/>
+        <c:axId val="121317632"/>
+        <c:axId val="121331712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83900672"/>
+        <c:axId val="121317632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1677,12 +1683,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83918848"/>
+        <c:crossAx val="121331712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83918848"/>
+        <c:axId val="121331712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,13 +1699,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83900672"/>
+        <c:crossAx val="121317632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2477,11 +2484,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84039168"/>
-        <c:axId val="84040704"/>
+        <c:axId val="122230272"/>
+        <c:axId val="122231808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84039168"/>
+        <c:axId val="122230272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2491,12 +2498,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84040704"/>
+        <c:crossAx val="122231808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84040704"/>
+        <c:axId val="122231808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -2509,13 +2516,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84039168"/>
+        <c:crossAx val="122230272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3122,11 +3130,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84135936"/>
-        <c:axId val="84137472"/>
+        <c:axId val="126730240"/>
+        <c:axId val="126731776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84135936"/>
+        <c:axId val="126730240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3136,12 +3144,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84137472"/>
+        <c:crossAx val="126731776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84137472"/>
+        <c:axId val="126731776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="55"/>
@@ -3153,13 +3161,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84135936"/>
+        <c:crossAx val="126730240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3189,6 +3198,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3286,11 +3296,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84165760"/>
-        <c:axId val="84167296"/>
+        <c:axId val="126895232"/>
+        <c:axId val="126896768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84165760"/>
+        <c:axId val="126895232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3300,12 +3310,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84167296"/>
+        <c:crossAx val="126896768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84167296"/>
+        <c:axId val="126896768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20"/>
@@ -3317,13 +3327,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84165760"/>
+        <c:crossAx val="126895232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3353,6 +3364,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3450,11 +3462,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84195968"/>
-        <c:axId val="84205952"/>
+        <c:axId val="126925440"/>
+        <c:axId val="126935424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84195968"/>
+        <c:axId val="126925440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3464,12 +3476,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84205952"/>
+        <c:crossAx val="126935424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84205952"/>
+        <c:axId val="126935424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-1500"/>
@@ -3481,13 +3493,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84195968"/>
+        <c:crossAx val="126925440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3517,6 +3530,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3614,11 +3628,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84685184"/>
-        <c:axId val="84686720"/>
+        <c:axId val="127222144"/>
+        <c:axId val="127223680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84685184"/>
+        <c:axId val="127222144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3628,12 +3642,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84686720"/>
+        <c:crossAx val="127223680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84686720"/>
+        <c:axId val="127223680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3644,13 +3658,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84685184"/>
+        <c:crossAx val="127222144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4352,11 +4367,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84316544"/>
-        <c:axId val="84318080"/>
+        <c:axId val="128033152"/>
+        <c:axId val="128034688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84316544"/>
+        <c:axId val="128033152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -4368,12 +4383,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84318080"/>
+        <c:crossAx val="128034688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84318080"/>
+        <c:axId val="128034688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -4386,13 +4401,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84316544"/>
+        <c:crossAx val="128033152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4543,11 +4559,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67387776"/>
-        <c:axId val="67389312"/>
+        <c:axId val="117215232"/>
+        <c:axId val="117216768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67387776"/>
+        <c:axId val="117215232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4557,12 +4573,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67389312"/>
+        <c:crossAx val="117216768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67389312"/>
+        <c:axId val="117216768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -4575,7 +4591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67387776"/>
+        <c:crossAx val="117215232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5153,11 +5169,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84420864"/>
-        <c:axId val="84422656"/>
+        <c:axId val="128092416"/>
+        <c:axId val="128110592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84420864"/>
+        <c:axId val="128092416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5167,12 +5183,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84422656"/>
+        <c:crossAx val="128110592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84422656"/>
+        <c:axId val="128110592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="45"/>
@@ -5184,13 +5200,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84420864"/>
+        <c:crossAx val="128092416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5220,6 +5237,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5314,11 +5332,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84430208"/>
-        <c:axId val="84460672"/>
+        <c:axId val="128118144"/>
+        <c:axId val="128484480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84430208"/>
+        <c:axId val="128118144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5328,12 +5346,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84460672"/>
+        <c:crossAx val="128484480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84460672"/>
+        <c:axId val="128484480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5344,13 +5362,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84430208"/>
+        <c:crossAx val="128118144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5380,6 +5399,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5474,11 +5494,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84546688"/>
-        <c:axId val="84548224"/>
+        <c:axId val="128504960"/>
+        <c:axId val="128506496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84546688"/>
+        <c:axId val="128504960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5488,12 +5508,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84548224"/>
+        <c:crossAx val="128506496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84548224"/>
+        <c:axId val="128506496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-900"/>
@@ -5506,13 +5526,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84546688"/>
+        <c:crossAx val="128504960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5542,6 +5563,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5639,11 +5661,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84576896"/>
-        <c:axId val="84586880"/>
+        <c:axId val="128875136"/>
+        <c:axId val="128881024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84576896"/>
+        <c:axId val="128875136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5653,12 +5675,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84586880"/>
+        <c:crossAx val="128881024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84586880"/>
+        <c:axId val="128881024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="68"/>
@@ -5670,13 +5692,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84576896"/>
+        <c:crossAx val="128875136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6300,11 +6323,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84644992"/>
-        <c:axId val="84646528"/>
+        <c:axId val="128959616"/>
+        <c:axId val="128961152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84644992"/>
+        <c:axId val="128959616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70.5"/>
@@ -6316,12 +6339,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84646528"/>
+        <c:crossAx val="128961152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84646528"/>
+        <c:axId val="128961152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -6334,13 +6357,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84644992"/>
+        <c:crossAx val="128959616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7094,11 +7118,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84849408"/>
-        <c:axId val="84850944"/>
+        <c:axId val="129082112"/>
+        <c:axId val="129083648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84849408"/>
+        <c:axId val="129082112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7108,12 +7132,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84850944"/>
+        <c:crossAx val="129083648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84850944"/>
+        <c:axId val="129083648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="45"/>
@@ -7125,13 +7149,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84849408"/>
+        <c:crossAx val="129082112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7769,11 +7794,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84872192"/>
-        <c:axId val="84878080"/>
+        <c:axId val="129580032"/>
+        <c:axId val="129594112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84872192"/>
+        <c:axId val="129580032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7783,12 +7808,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84878080"/>
+        <c:crossAx val="129594112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84878080"/>
+        <c:axId val="129594112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -7801,7 +7826,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84872192"/>
+        <c:crossAx val="129580032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7814,6 +7839,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8510,11 +8536,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84866944"/>
-        <c:axId val="84868480"/>
+        <c:axId val="129775488"/>
+        <c:axId val="129777024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84866944"/>
+        <c:axId val="129775488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8524,12 +8550,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84868480"/>
+        <c:crossAx val="129777024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84868480"/>
+        <c:axId val="129777024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="45"/>
@@ -8541,13 +8567,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84866944"/>
+        <c:crossAx val="129775488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8577,6 +8604,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8674,11 +8702,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84917248"/>
-        <c:axId val="85144320"/>
+        <c:axId val="129797120"/>
+        <c:axId val="129807104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84917248"/>
+        <c:axId val="129797120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8688,12 +8716,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85144320"/>
+        <c:crossAx val="129807104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85144320"/>
+        <c:axId val="129807104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="37"/>
@@ -8706,13 +8734,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84917248"/>
+        <c:crossAx val="129797120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8742,6 +8771,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8839,11 +8869,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84951808"/>
-        <c:axId val="84953344"/>
+        <c:axId val="129975040"/>
+        <c:axId val="129976576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84951808"/>
+        <c:axId val="129975040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8853,12 +8883,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84953344"/>
+        <c:crossAx val="129976576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84953344"/>
+        <c:axId val="129976576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8869,13 +8899,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84951808"/>
+        <c:crossAx val="129975040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9517,11 +9548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67789952"/>
-        <c:axId val="67791488"/>
+        <c:axId val="118190848"/>
+        <c:axId val="118192384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67789952"/>
+        <c:axId val="118190848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9531,12 +9562,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67791488"/>
+        <c:crossAx val="118192384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67791488"/>
+        <c:axId val="118192384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -9548,7 +9579,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67789952"/>
+        <c:crossAx val="118190848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9585,6 +9616,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -9682,11 +9714,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84961536"/>
-        <c:axId val="84983808"/>
+        <c:axId val="129984768"/>
+        <c:axId val="130015232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84961536"/>
+        <c:axId val="129984768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9696,12 +9728,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84983808"/>
+        <c:crossAx val="130015232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84983808"/>
+        <c:axId val="130015232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9712,13 +9744,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84961536"/>
+        <c:crossAx val="129984768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10440,11 +10473,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85121280"/>
-        <c:axId val="85458944"/>
+        <c:axId val="130074880"/>
+        <c:axId val="130088960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85121280"/>
+        <c:axId val="130074880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="71.5"/>
@@ -10456,12 +10489,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85458944"/>
+        <c:crossAx val="130088960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85458944"/>
+        <c:axId val="130088960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -10474,13 +10507,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85121280"/>
+        <c:crossAx val="130074880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10926,11 +10960,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85204352"/>
-        <c:axId val="85226624"/>
+        <c:axId val="130129280"/>
+        <c:axId val="130139264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85204352"/>
+        <c:axId val="130129280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10940,12 +10974,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85226624"/>
+        <c:crossAx val="130139264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85226624"/>
+        <c:axId val="130139264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="22"/>
@@ -10957,7 +10991,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85204352"/>
+        <c:crossAx val="130129280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11400,11 +11434,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85254144"/>
-        <c:axId val="85255680"/>
+        <c:axId val="130306048"/>
+        <c:axId val="130307584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85254144"/>
+        <c:axId val="130306048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11414,12 +11448,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85255680"/>
+        <c:crossAx val="130307584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85255680"/>
+        <c:axId val="130307584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11430,7 +11464,778 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85254144"/>
+        <c:crossAx val="130306048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>vs!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>264.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.1776535013042424"/>
+                  <c:y val="-1.2512051151385692E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>vs!$B$34:$B$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>71.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>71.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>71.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>72.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>72.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>vs!$C$34:$C$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>69.09253600000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.196194999999989</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.843277999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77.027042000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80.126172499999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.515842500000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85.379997500000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.235012499999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.011347499999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>92.944536666666679</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>94.832933999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>99.048960000000008</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100.05341200000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>105.05459666666667</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>104.89112999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>107.64413999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>vs!$F$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>285</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.37871150866270187"/>
+                  <c:y val="0.18975667768557136"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>vs!$G$34:$G$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>vs!$H$34:$H$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>52.89312000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58.384426857142849</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63.805609999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66.414344</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68.44764185714287</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>74.014818571428577</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76.311572857142863</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>79.583640000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>vs!$K$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>290</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.17932285290145714"/>
+                  <c:y val="-3.9198073126252585E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>vs!$L$34:$L$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>vs!$M$34:$M$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>61.741945666666673</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63.851516000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.487919857142856</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.990085714285712</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71.46619577777777</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>74.471741249999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>78.828692857142855</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>vs!$P$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>305</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.17408788126379371"/>
+                  <c:y val="0.20132161332490262"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>vs!$Q$34:$Q$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>vs!$R$34:$R$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52.382251500000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.138100000000009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.464179999999985</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61.728080399999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63.333358333333329</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65.05206714285714</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68.753920375000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.107734285714287</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72.172114999999991</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>vs!$U$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>310</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.4326010827564226E-2"/>
+                  <c:y val="0.19088785526883637"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>vs!$V$34:$V$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>72.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>73.099999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>vs!$W$34:$W$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>57.237031666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61.227995857142851</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.699667500000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66.076822499999992</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.265810000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>73.502705000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74.355491428571426</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78.367583750000009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="120661120"/>
+        <c:axId val="120659328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="120661120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120659328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="120659328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120661120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>vs!$O$46:$O$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>264.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>310</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>vs!$P$46:$P$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>68.040208717004305</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.974720707667672</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69.072409834118531</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69.49053987565415</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.466756212222961</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="135958912"/>
+        <c:axId val="135902336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="135958912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="135902336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="135902336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="135958912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12582,11 +13387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67987328"/>
-        <c:axId val="68001792"/>
+        <c:axId val="118281728"/>
+        <c:axId val="118283648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67987328"/>
+        <c:axId val="118281728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12596,12 +13401,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68001792"/>
+        <c:crossAx val="118283648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68001792"/>
+        <c:axId val="118283648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -12613,7 +13418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67987328"/>
+        <c:crossAx val="118281728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12736,11 +13541,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69533696"/>
-        <c:axId val="69535232"/>
+        <c:axId val="118377856"/>
+        <c:axId val="118391936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69533696"/>
+        <c:axId val="118377856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12750,12 +13555,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69535232"/>
+        <c:crossAx val="118391936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69535232"/>
+        <c:axId val="118391936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12766,7 +13571,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69533696"/>
+        <c:crossAx val="118377856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12889,11 +13694,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69547520"/>
-        <c:axId val="69549056"/>
+        <c:axId val="118629504"/>
+        <c:axId val="118631040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69547520"/>
+        <c:axId val="118629504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12903,12 +13708,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69549056"/>
+        <c:crossAx val="118631040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69549056"/>
+        <c:axId val="118631040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12919,7 +13724,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69547520"/>
+        <c:crossAx val="118629504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12956,6 +13761,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -13041,11 +13847,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="69577344"/>
-        <c:axId val="69583232"/>
+        <c:axId val="118651520"/>
+        <c:axId val="118657408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69577344"/>
+        <c:axId val="118651520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13055,12 +13861,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69583232"/>
+        <c:crossAx val="118657408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69583232"/>
+        <c:axId val="118657408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13071,13 +13877,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69577344"/>
+        <c:crossAx val="118651520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13796,11 +14603,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74222976"/>
-        <c:axId val="74241152"/>
+        <c:axId val="118795648"/>
+        <c:axId val="118805632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74222976"/>
+        <c:axId val="118795648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="69"/>
@@ -13812,12 +14619,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74241152"/>
+        <c:crossAx val="118805632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74241152"/>
+        <c:axId val="118805632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30"/>
@@ -13830,7 +14637,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74222976"/>
+        <c:crossAx val="118795648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14486,11 +15293,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74585984"/>
-        <c:axId val="74587520"/>
+        <c:axId val="119175040"/>
+        <c:axId val="119176576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74585984"/>
+        <c:axId val="119175040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14500,12 +15307,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74587520"/>
+        <c:crossAx val="119176576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74587520"/>
+        <c:axId val="119176576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
@@ -14517,13 +15324,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74585984"/>
+        <c:crossAx val="119175040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14794,16 +15602,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14824,13 +15632,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
@@ -14860,7 +15668,7 @@
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
@@ -14884,13 +15692,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
@@ -14914,13 +15722,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>33337</xdr:rowOff>
@@ -14950,7 +15758,7 @@
       <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>504824</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -15134,16 +15942,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>176211</xdr:rowOff>
+      <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>466724</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15254,16 +16062,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>166686</xdr:rowOff>
+      <xdr:rowOff>157161</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15284,16 +16092,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>109536</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>400049</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15319,16 +16127,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>33336</xdr:rowOff>
+      <xdr:rowOff>128586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15349,16 +16157,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>33336</xdr:rowOff>
+      <xdr:rowOff>80961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>438149</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15557,6 +16365,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -15854,8 +16722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16813,8 +17681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17203,15 +18071,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -17248,8 +18116,11 @@
       <c r="L1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>72</v>
       </c>
@@ -17283,8 +18154,12 @@
       <c r="K2">
         <v>78.628000000000043</v>
       </c>
+      <c r="N2">
+        <f>AVERAGE(B2:L2)</f>
+        <v>79.583640000000003</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>71.900000000000006</v>
       </c>
@@ -17309,8 +18184,12 @@
       <c r="H3">
         <v>74.55600000000004</v>
       </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N9" si="0">AVERAGE(B3:L3)</f>
+        <v>76.311572857142863</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>71.8</v>
       </c>
@@ -17335,8 +18214,12 @@
       <c r="H4">
         <v>71.734999999999999</v>
       </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>74.014818571428577</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>71.599999999999994</v>
       </c>
@@ -17361,8 +18244,12 @@
       <c r="H5">
         <v>66.134000000000015</v>
       </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>68.44764185714287</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>71.5</v>
       </c>
@@ -17396,8 +18283,12 @@
       <c r="K6">
         <v>64.045000000000002</v>
       </c>
+      <c r="N6">
+        <f>AVERAGE(B6:L6)</f>
+        <v>66.414344</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>71.400000000000006</v>
       </c>
@@ -17422,8 +18313,12 @@
       <c r="H7">
         <v>63.652999999999963</v>
       </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>63.805609999999994</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>71.2</v>
       </c>
@@ -17448,8 +18343,12 @@
       <c r="H8">
         <v>57.265999999999963</v>
       </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>58.384426857142849</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>71</v>
       </c>
@@ -17471,8 +18370,12 @@
       <c r="G9">
         <v>50.692000000000007</v>
       </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>52.89312000000001</v>
+      </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0</v>
       </c>
@@ -17504,7 +18407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -17530,7 +18433,7 @@
         <v>25.428999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -17562,7 +18465,7 @@
         <v>-1753</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -17571,27 +18474,27 @@
         <v>69.134221311475414</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:H16" si="0">-C15/C14</f>
+        <f t="shared" ref="C16:H16" si="1">-C15/C14</f>
         <v>68.85378852243764</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68.975745287977773</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68.908871501420847</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68.937040386959779</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.126051031922245</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68.937040386959779</v>
       </c>
     </row>
@@ -17609,15 +18512,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -17654,8 +18557,11 @@
       <c r="L1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>72.2</v>
       </c>
@@ -17680,8 +18586,12 @@
       <c r="H2">
         <v>77.336999999999989</v>
       </c>
+      <c r="N2">
+        <f>AVERAGE(B2:L2)</f>
+        <v>78.828692857142855</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>72</v>
       </c>
@@ -17709,8 +18619,12 @@
       <c r="I3">
         <v>73.045000000000002</v>
       </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N8" si="0">AVERAGE(B3:L3)</f>
+        <v>74.471741249999994</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>71.900000000000006</v>
       </c>
@@ -17741,8 +18655,12 @@
       <c r="J4">
         <v>71.385999999999967</v>
       </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>71.46619577777777</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>71.8</v>
       </c>
@@ -17767,8 +18685,12 @@
       <c r="H5">
         <v>67.09899999999999</v>
       </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>68.990085714285712</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>71.7</v>
       </c>
@@ -17793,8 +18715,12 @@
       <c r="H6">
         <v>64.43199999999996</v>
       </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>65.487919857142856</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>71.599999999999994</v>
       </c>
@@ -17819,8 +18745,12 @@
       <c r="H7">
         <v>62.291999999999973</v>
       </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>63.851516000000004</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>71.5</v>
       </c>
@@ -17842,8 +18772,12 @@
       <c r="G8">
         <v>61.25200000000001</v>
       </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>61.741945666666673</v>
+      </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0</v>
       </c>
@@ -17866,7 +18800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -17892,7 +18826,7 @@
         <v>26.207000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -17925,36 +18859,36 @@
         <v>-1814.1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:H16" si="0">-B15/B14</f>
+        <f t="shared" ref="B16:H16" si="1">-B15/B14</f>
         <v>69.166929133858275</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.130004036252885</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.308870680441757</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68.822746209680886</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.121371517631019</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68.975391127526237</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.221963597512115</v>
       </c>
     </row>
@@ -17972,15 +18906,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -18017,8 +18951,11 @@
       <c r="L1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>72.8</v>
       </c>
@@ -18028,8 +18965,12 @@
       <c r="C2">
         <v>74.842899999999986</v>
       </c>
+      <c r="N2">
+        <f>AVERAGE(B2:L2)</f>
+        <v>72.172114999999991</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>72.599999999999994</v>
       </c>
@@ -18054,8 +18995,12 @@
       <c r="H3">
         <v>68.22399999999999</v>
       </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N10" si="0">AVERAGE(B3:L3)</f>
+        <v>70.107734285714287</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>72.5</v>
       </c>
@@ -18083,8 +19028,12 @@
       <c r="I4">
         <v>67.692000000000064</v>
       </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>68.753920375000007</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>72.400000000000006</v>
       </c>
@@ -18109,8 +19058,12 @@
       <c r="H5">
         <v>62.238999999999976</v>
       </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>65.05206714285714</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>72.3</v>
       </c>
@@ -18132,8 +19085,12 @@
       <c r="G6">
         <v>63.812999999999988</v>
       </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>63.333358333333329</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>72.2</v>
       </c>
@@ -18152,8 +19109,12 @@
       <c r="F7">
         <v>60.727000000000004</v>
       </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>61.728080399999996</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>72.099999999999994</v>
       </c>
@@ -18172,8 +19133,12 @@
       <c r="F8">
         <v>57.18199999999996</v>
       </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>58.464179999999985</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>72</v>
       </c>
@@ -18189,8 +19154,12 @@
       <c r="E9">
         <v>55.406000000000006</v>
       </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>56.138100000000009</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>71.900000000000006</v>
       </c>
@@ -18206,8 +19175,12 @@
       <c r="E10">
         <v>52.300000000000011</v>
       </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>52.382251500000002</v>
+      </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0</v>
       </c>
@@ -18233,7 +19206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -18256,7 +19229,7 @@
         <v>20.023</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -18285,32 +19258,32 @@
         <v>-1384.4</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:G16" si="0">-B15/B14</f>
+        <f t="shared" ref="B16:G16" si="1">-B15/B14</f>
         <v>69.79766339315951</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.311129961158983</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.945874780573433</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.931926989826451</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.628675681476707</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.140488438295961</v>
       </c>
     </row>
@@ -18331,15 +19304,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -18367,8 +19340,11 @@
       <c r="I1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>73.099999999999994</v>
       </c>
@@ -18396,8 +19372,12 @@
       <c r="I2">
         <v>76.900999999999954</v>
       </c>
+      <c r="K2">
+        <f>AVERAGE(B2:I2)</f>
+        <v>78.367583750000009</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>73</v>
       </c>
@@ -18422,8 +19402,12 @@
       <c r="H3">
         <v>72.548000000000002</v>
       </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K9" si="0">AVERAGE(B3:I3)</f>
+        <v>74.355491428571426</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>72.900000000000006</v>
       </c>
@@ -18445,8 +19429,12 @@
       <c r="G4">
         <v>72.038999999999987</v>
       </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>73.502705000000006</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>72.8</v>
       </c>
@@ -18474,8 +19462,12 @@
       <c r="I5">
         <v>68.317999999999984</v>
       </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>70.265810000000002</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>72.7</v>
       </c>
@@ -18491,8 +19483,12 @@
       <c r="E6">
         <v>66.972999999999985</v>
       </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>66.076822499999992</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>72.599999999999994</v>
       </c>
@@ -18508,8 +19504,12 @@
       <c r="E7">
         <v>63.814999999999998</v>
       </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>62.699667500000004</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>72.5</v>
       </c>
@@ -18534,8 +19534,12 @@
       <c r="H8">
         <v>59.531000000000006</v>
       </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>61.227995857142851</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>72.400000000000006</v>
       </c>
@@ -18557,8 +19561,12 @@
       <c r="G9">
         <v>51.331999999999994</v>
       </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>57.237031666666667</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0</v>
       </c>
@@ -18584,7 +19592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -18607,7 +19615,7 @@
         <v>35.32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -18636,32 +19644,32 @@
         <v>-2503.4</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:G16" si="0">-B15/B14</f>
+        <f t="shared" ref="B16:G16" si="1">-B15/B14</f>
         <v>70.684740609362137</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70.267089826338122</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70.175826606214741</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70.464940278371884</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70.31911487423956</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70.877689694224244</v>
       </c>
     </row>
@@ -18682,10 +19690,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T7"/>
+  <dimension ref="A2:X50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="N68" sqref="N68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18996,7 +20004,470 @@
         <v>70.877689694224244</v>
       </c>
     </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" t="s">
+        <v>0</v>
+      </c>
+      <c r="L33" t="s">
+        <v>1</v>
+      </c>
+      <c r="M33" t="s">
+        <v>13</v>
+      </c>
+      <c r="N33" t="s">
+        <v>16</v>
+      </c>
+      <c r="P33" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>1</v>
+      </c>
+      <c r="R33" t="s">
+        <v>13</v>
+      </c>
+      <c r="S33" t="s">
+        <v>16</v>
+      </c>
+      <c r="U33" t="s">
+        <v>0</v>
+      </c>
+      <c r="V33" t="s">
+        <v>1</v>
+      </c>
+      <c r="W33" t="s">
+        <v>13</v>
+      </c>
+      <c r="X33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>264.5</v>
+      </c>
+      <c r="B34">
+        <v>70.7</v>
+      </c>
+      <c r="C34">
+        <v>69.09253600000001</v>
+      </c>
+      <c r="D34">
+        <f>1773.4/26.064</f>
+        <v>68.040208717004305</v>
+      </c>
+      <c r="F34">
+        <v>285</v>
+      </c>
+      <c r="G34">
+        <v>71</v>
+      </c>
+      <c r="H34">
+        <v>52.89312000000001</v>
+      </c>
+      <c r="I34">
+        <f>1809/26.227</f>
+        <v>68.974720707667672</v>
+      </c>
+      <c r="K34">
+        <v>290</v>
+      </c>
+      <c r="L34">
+        <v>71.5</v>
+      </c>
+      <c r="M34">
+        <v>61.741945666666673</v>
+      </c>
+      <c r="N34">
+        <f>1744.7/25.259</f>
+        <v>69.072409834118531</v>
+      </c>
+      <c r="P34">
+        <v>305</v>
+      </c>
+      <c r="Q34">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="R34">
+        <v>52.382251500000002</v>
+      </c>
+      <c r="S34">
+        <f>1553.6/22.357</f>
+        <v>69.49053987565415</v>
+      </c>
+      <c r="U34">
+        <v>310</v>
+      </c>
+      <c r="V34">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="W34">
+        <v>57.237031666666667</v>
+      </c>
+      <c r="X34">
+        <f>2098.5/29.78</f>
+        <v>70.466756212222961</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>70.8</v>
+      </c>
+      <c r="C35">
+        <v>72.196194999999989</v>
+      </c>
+      <c r="G35">
+        <v>71.2</v>
+      </c>
+      <c r="H35">
+        <v>58.384426857142849</v>
+      </c>
+      <c r="L35">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="M35">
+        <v>63.851516000000004</v>
+      </c>
+      <c r="Q35">
+        <v>72</v>
+      </c>
+      <c r="R35">
+        <v>56.138100000000009</v>
+      </c>
+      <c r="V35">
+        <v>72.5</v>
+      </c>
+      <c r="W35">
+        <v>61.227995857142851</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="C36">
+        <v>73.843277999999998</v>
+      </c>
+      <c r="G36">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="H36">
+        <v>63.805609999999994</v>
+      </c>
+      <c r="L36">
+        <v>71.7</v>
+      </c>
+      <c r="M36">
+        <v>65.487919857142856</v>
+      </c>
+      <c r="Q36">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="R36">
+        <v>58.464179999999985</v>
+      </c>
+      <c r="V36">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="W36">
+        <v>62.699667500000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>71</v>
+      </c>
+      <c r="C37">
+        <v>77.027042000000009</v>
+      </c>
+      <c r="G37">
+        <v>71.5</v>
+      </c>
+      <c r="H37">
+        <v>66.414344</v>
+      </c>
+      <c r="L37">
+        <v>71.8</v>
+      </c>
+      <c r="M37">
+        <v>68.990085714285712</v>
+      </c>
+      <c r="Q37">
+        <v>72.2</v>
+      </c>
+      <c r="R37">
+        <v>61.728080399999996</v>
+      </c>
+      <c r="V37">
+        <v>72.7</v>
+      </c>
+      <c r="W37">
+        <v>66.076822499999992</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="C38">
+        <v>80.126172499999996</v>
+      </c>
+      <c r="G38">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="H38">
+        <v>68.44764185714287</v>
+      </c>
+      <c r="L38">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="M38">
+        <v>71.46619577777777</v>
+      </c>
+      <c r="Q38">
+        <v>72.3</v>
+      </c>
+      <c r="R38">
+        <v>63.333358333333329</v>
+      </c>
+      <c r="V38">
+        <v>72.8</v>
+      </c>
+      <c r="W38">
+        <v>70.265810000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>71.2</v>
+      </c>
+      <c r="C39">
+        <v>82.515842500000005</v>
+      </c>
+      <c r="G39">
+        <v>71.8</v>
+      </c>
+      <c r="H39">
+        <v>74.014818571428577</v>
+      </c>
+      <c r="L39">
+        <v>72</v>
+      </c>
+      <c r="M39">
+        <v>74.471741249999994</v>
+      </c>
+      <c r="Q39">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="R39">
+        <v>65.05206714285714</v>
+      </c>
+      <c r="V39">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="W39">
+        <v>73.502705000000006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>71.3</v>
+      </c>
+      <c r="C40">
+        <v>85.379997500000002</v>
+      </c>
+      <c r="G40">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="H40">
+        <v>76.311572857142863</v>
+      </c>
+      <c r="L40">
+        <v>72.2</v>
+      </c>
+      <c r="M40">
+        <v>78.828692857142855</v>
+      </c>
+      <c r="Q40">
+        <v>72.5</v>
+      </c>
+      <c r="R40">
+        <v>68.753920375000007</v>
+      </c>
+      <c r="V40">
+        <v>73</v>
+      </c>
+      <c r="W40">
+        <v>74.355491428571426</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="C41">
+        <v>88.235012499999996</v>
+      </c>
+      <c r="G41">
+        <v>72</v>
+      </c>
+      <c r="H41">
+        <v>79.583640000000003</v>
+      </c>
+      <c r="Q41">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="R41">
+        <v>70.107734285714287</v>
+      </c>
+      <c r="V41">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="W41">
+        <v>78.367583750000009</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>71.5</v>
+      </c>
+      <c r="C42">
+        <v>90.011347499999999</v>
+      </c>
+      <c r="Q42">
+        <v>72.8</v>
+      </c>
+      <c r="R42">
+        <v>72.172114999999991</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="C43">
+        <v>92.944536666666679</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>71.7</v>
+      </c>
+      <c r="C44">
+        <v>94.832933999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>71.8</v>
+      </c>
+      <c r="C45">
+        <v>99.048960000000008</v>
+      </c>
+      <c r="O45" t="s">
+        <v>0</v>
+      </c>
+      <c r="P45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="C46">
+        <v>100.05341200000001</v>
+      </c>
+      <c r="O46">
+        <v>264.5</v>
+      </c>
+      <c r="P46">
+        <f>D34</f>
+        <v>68.040208717004305</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>72</v>
+      </c>
+      <c r="C47">
+        <v>105.05459666666667</v>
+      </c>
+      <c r="O47">
+        <v>285</v>
+      </c>
+      <c r="P47">
+        <f>I34</f>
+        <v>68.974720707667672</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="C48">
+        <v>104.89112999999998</v>
+      </c>
+      <c r="O48">
+        <v>290</v>
+      </c>
+      <c r="P48">
+        <f>N34</f>
+        <v>69.072409834118531</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>72.2</v>
+      </c>
+      <c r="C49">
+        <v>107.64413999999999</v>
+      </c>
+      <c r="O49">
+        <v>305</v>
+      </c>
+      <c r="P49">
+        <f>S34</f>
+        <v>69.49053987565415</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O50">
+        <v>310</v>
+      </c>
+      <c r="P50">
+        <f>X34</f>
+        <v>70.466756212222961</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="V34:W42">
+    <sortCondition ref="V34"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>